<commit_message>
Data .xsl and App update
- Add new tab: analysis of consumption. The Observatory of Drugs in Colombia doesn't count with much information about the consumption of drugs in Colombia. However, I decided to few of it's variables, so that the app can provide a general understanding of the drug market in Colombia.
- Additional changes in the structure of the app before adding the plots/tab already created.
</commit_message>
<xml_diff>
--- a/data_xls/obs_drug_colombia.xlsx
+++ b/data_xls/obs_drug_colombia.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgoye\OneDrive\Documents\GitHub\project1_lgoyenec\data_xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="8_{D1329E90-7AED-4578-A970-877C7302D35D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{FC2546C5-84DB-40EE-9ADC-0C4CE2C86CFE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310C1BDF-36B5-4998-AE60-90580BC0F90E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F581D121-48E3-4EB7-819A-93A2A7DA1688}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{F581D121-48E3-4EB7-819A-93A2A7DA1688}"/>
   </bookViews>
   <sheets>
     <sheet name="illicit_crops" sheetId="1" r:id="rId1"/>
     <sheet name="manual_eradication" sheetId="2" r:id="rId2"/>
     <sheet name="seizures" sheetId="3" r:id="rId3"/>
+    <sheet name="criminality" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="35">
   <si>
     <t>Year</t>
   </si>
@@ -66,13 +67,85 @@
   </si>
   <si>
     <t>Cocaine Hydrochloride</t>
+  </si>
+  <si>
+    <t>TRAFICO FABRICACION O PORTE DE ESTUPEFACIENTES</t>
+  </si>
+  <si>
+    <t>LAVADO DE ACTIVOS</t>
+  </si>
+  <si>
+    <t>DESTINACION ILICITA DE MUEBLES O INMUEBLES</t>
+  </si>
+  <si>
+    <t>TRAFICO DE SUSTANCIAS PARA PROCESAMIENTO DE NARCOTICOS</t>
+  </si>
+  <si>
+    <t>CONSERVACION O FINANCIACION DE PLANTACIONES</t>
+  </si>
+  <si>
+    <t>Tema</t>
+  </si>
+  <si>
+    <t>Desagregacion</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>CONDENADO</t>
+  </si>
+  <si>
+    <t>SINDICADO</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t>Crime</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Convicted</t>
+  </si>
+  <si>
+    <t>Accused</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Narcotics trafficking, manufacture and possession</t>
+  </si>
+  <si>
+    <t>crime_code</t>
+  </si>
+  <si>
+    <t>Money laundering</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Use of storage unit for illicit activites</t>
+  </si>
+  <si>
+    <t>Traffick of ingredients for drugs purposes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +179,10 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -124,10 +201,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -150,9 +228,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{FCA2298B-4F90-4489-B3F3-19CDF1FC6018}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -843,7 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B051E0-A995-4FE8-BE6A-AE5D222970BB}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1713,4 +1798,666 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1A74D6-370B-4AC6-8F28-994E4AD39B41}">
+  <dimension ref="A1:G179"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="56.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.33203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="7" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="9">
+        <v>16743</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="9">
+        <v>7821</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="9">
+        <v>20922</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="9">
+        <v>3642</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="9">
+        <v>2</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="9">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="9">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="9">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="9">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="9">
+        <v>3</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="9">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="9">
+        <v>3</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="9">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="9">
+        <v>3</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="9">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="9">
+        <v>3</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="9">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="9">
+        <v>4</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="9">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="9">
+        <v>4</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="9">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="9">
+        <v>4</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="9">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="9">
+        <v>4</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="9">
+        <v>5</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="9">
+        <v>5</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="9">
+        <v>5</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="9">
+        <v>5</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="128" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="129" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="130" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="131" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="132" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="133" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="134" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="135" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="136" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="137" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="138" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="139" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="140" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="141" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="142" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="143" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="146" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="147" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="149" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="160" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="161" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="162" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="163" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="164" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="165" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="167" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="168" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="169" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="170" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="172" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="173" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="174" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="176" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="177" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="178" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="179" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
+    <sortCondition ref="D2:D21"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding reactive / observe
From draft script and markdown in R, I'm organizing the data n a way that create interactive plots and data sets; meaning that depend on the conditional sidebar options.
</commit_message>
<xml_diff>
--- a/data_xls/obs_drug_colombia.xlsx
+++ b/data_xls/obs_drug_colombia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgoye\OneDrive\Documents\GitHub\project1_lgoyenec\data_xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310C1BDF-36B5-4998-AE60-90580BC0F90E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="114_{8E06FA86-3850-4C52-A485-10A44CB47D89}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{F2AFC649-377B-474D-9040-0232E3AD31BC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{F581D121-48E3-4EB7-819A-93A2A7DA1688}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F581D121-48E3-4EB7-819A-93A2A7DA1688}"/>
   </bookViews>
   <sheets>
     <sheet name="illicit_crops" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Total Coca</t>
-  </si>
-  <si>
     <t xml:space="preserve">base de cocaina </t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Traffick of ingredients for drugs purposes</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70AB46DD-20D3-440B-99F9-91FE58E5B111}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -740,7 +740,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,7 +753,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -946,13 +946,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -963,10 +963,10 @@
         <v>16353.53</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -977,10 +977,10 @@
         <v>16939.259999999998</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -991,10 +991,10 @@
         <v>16623.27</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1005,10 +1005,10 @@
         <v>23595.25</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1019,10 +1019,10 @@
         <v>29470.59</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1033,10 +1033,10 @@
         <v>38401.589999999997</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1047,10 +1047,10 @@
         <v>54398.61</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1061,10 +1061,10 @@
         <v>50410.68</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1075,10 +1075,10 @@
         <v>63867.33</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1089,10 +1089,10 @@
         <v>54664.07</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1103,10 +1103,10 @@
         <v>53429.59</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1117,10 +1117,10 @@
         <v>106822.36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1131,10 +1131,10 @@
         <v>57100.55</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1145,10 +1145,10 @@
         <v>56053.55</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1159,10 +1159,10 @@
         <v>46621.5</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1173,10 +1173,10 @@
         <v>40890.15</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1187,10 +1187,10 @@
         <v>42657.54</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1201,10 +1201,10 @@
         <v>43073.440000000002</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1215,10 +1215,10 @@
         <v>52421.1</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1229,10 +1229,10 @@
         <v>42387.12</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1243,10 +1243,10 @@
         <v>306782</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1257,10 +1257,10 @@
         <v>897911.5</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1271,10 +1271,10 @@
         <v>583165.07999999996</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1285,10 +1285,10 @@
         <v>368000.63</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1299,10 +1299,10 @@
         <v>688690.51</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1313,10 +1313,10 @@
         <v>562263.56999999995</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1327,10 +1327,10 @@
         <v>665250.98</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1341,10 +1341,10 @@
         <v>844030.98</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1355,10 +1355,10 @@
         <v>1095840.54</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1369,10 +1369,10 @@
         <v>644353.49</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1383,10 +1383,10 @@
         <v>852778.57</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1397,10 +1397,10 @@
         <v>853136.82</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1411,10 +1411,10 @@
         <v>1023579.42</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1425,10 +1425,10 @@
         <v>481674.23</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1439,10 +1439,10 @@
         <v>446289.52</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1453,10 +1453,10 @@
         <v>532989.14</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1467,10 +1467,10 @@
         <v>777640.24</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1481,10 +1481,10 @@
         <v>1040878.24</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1495,10 +1495,10 @@
         <v>611412.86</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1509,10 +1509,10 @@
         <v>458429.33</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1523,10 +1523,10 @@
         <v>43632.72</v>
       </c>
       <c r="C42" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1537,10 +1537,10 @@
         <v>87268.84</v>
       </c>
       <c r="C43" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1551,10 +1551,10 @@
         <v>57240.29</v>
       </c>
       <c r="C44" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1565,10 +1565,10 @@
         <v>95278.07</v>
       </c>
       <c r="C45" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1579,10 +1579,10 @@
         <v>113142.24</v>
       </c>
       <c r="C46" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1593,10 +1593,10 @@
         <v>149297.22</v>
       </c>
       <c r="C47" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1607,10 +1607,10 @@
         <v>168465.18</v>
       </c>
       <c r="C48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1621,10 +1621,10 @@
         <v>130916.47</v>
       </c>
       <c r="C49" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1635,10 +1635,10 @@
         <v>131431.54999999999</v>
       </c>
       <c r="C50" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1649,10 +1649,10 @@
         <v>200983.5</v>
       </c>
       <c r="C51" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1663,10 +1663,10 @@
         <v>200017.51</v>
       </c>
       <c r="C52" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1677,10 +1677,10 @@
         <v>157148.04</v>
       </c>
       <c r="C53" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1691,10 +1691,10 @@
         <v>155557.71</v>
       </c>
       <c r="C54" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1705,10 +1705,10 @@
         <v>183245.39</v>
       </c>
       <c r="C55" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1719,10 +1719,10 @@
         <v>166981.76000000001</v>
       </c>
       <c r="C56" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1733,10 +1733,10 @@
         <v>148076.87</v>
       </c>
       <c r="C57" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1747,10 +1747,10 @@
         <v>253591.14</v>
       </c>
       <c r="C58" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1761,10 +1761,10 @@
         <v>362414.9</v>
       </c>
       <c r="C59" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1775,10 +1775,10 @@
         <v>434729.75</v>
       </c>
       <c r="C60" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1789,10 +1789,10 @@
         <v>413383.28</v>
       </c>
       <c r="C61" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1804,7 +1804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1A74D6-370B-4AC6-8F28-994E4AD39B41}">
   <dimension ref="A1:G179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -1825,22 +1825,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1848,19 +1848,19 @@
         <v>2018</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="9">
         <v>1</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="9">
         <v>16743</v>
@@ -1871,19 +1871,19 @@
         <v>2018</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="9">
         <v>1</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="9">
         <v>7821</v>
@@ -1894,19 +1894,19 @@
         <v>2018</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="9">
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="9">
         <v>20922</v>
@@ -1917,19 +1917,19 @@
         <v>2018</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="9">
         <v>1</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="9">
         <v>3642</v>
@@ -1940,19 +1940,19 @@
         <v>2018</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="9">
         <v>2</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="9">
         <v>568</v>
@@ -1963,19 +1963,19 @@
         <v>2018</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="9">
         <v>2</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="9">
         <v>323</v>
@@ -1986,19 +1986,19 @@
         <v>2018</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="9">
         <v>2</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="9">
         <v>637</v>
@@ -2009,19 +2009,19 @@
         <v>2018</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="9">
         <v>2</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="9">
         <v>254</v>
@@ -2032,19 +2032,19 @@
         <v>2018</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="9">
         <v>3</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G10" s="9">
         <v>164</v>
@@ -2055,19 +2055,19 @@
         <v>2018</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="9">
         <v>3</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="9">
         <v>130</v>
@@ -2078,19 +2078,19 @@
         <v>2018</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="9">
         <v>3</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="9">
         <v>226</v>
@@ -2101,19 +2101,19 @@
         <v>2018</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="9">
         <v>3</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" s="9">
         <v>68</v>
@@ -2124,19 +2124,19 @@
         <v>2018</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="9">
         <v>4</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G14" s="9">
         <v>269</v>
@@ -2147,19 +2147,19 @@
         <v>2018</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="9">
         <v>4</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15" s="9">
         <v>144</v>
@@ -2170,19 +2170,19 @@
         <v>2018</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="9">
         <v>4</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G16" s="9">
         <v>391</v>
@@ -2193,19 +2193,19 @@
         <v>2018</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="9">
         <v>4</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="9">
         <v>22</v>
@@ -2216,19 +2216,19 @@
         <v>2018</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="9">
         <v>5</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G18" s="9">
         <v>41</v>
@@ -2239,19 +2239,19 @@
         <v>2018</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="9">
         <v>5</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G19" s="9">
         <v>19</v>
@@ -2262,19 +2262,19 @@
         <v>2018</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="9">
         <v>5</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G20" s="9">
         <v>57</v>
@@ -2285,19 +2285,19 @@
         <v>2018</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="9">
         <v>5</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G21" s="9">
         <v>3</v>

</xml_diff>

<commit_message>
Additional changes in app and data .xls
More details to app:
- Change colors, title
- Add 2 additional valuebox
- Due to lack of time, eliminate tab "Consumption"

Data .xls:
- Add categorical variable in sheet criminality
</commit_message>
<xml_diff>
--- a/data_xls/obs_drug_colombia.xlsx
+++ b/data_xls/obs_drug_colombia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgoye\OneDrive\Documents\GitHub\project1_lgoyenec\data_xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="114_{8E06FA86-3850-4C52-A485-10A44CB47D89}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{F2AFC649-377B-474D-9040-0232E3AD31BC}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="114_{8E06FA86-3850-4C52-A485-10A44CB47D89}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{252BB60C-B8AD-4D18-8C0B-2D4A42B28185}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F581D121-48E3-4EB7-819A-93A2A7DA1688}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{F581D121-48E3-4EB7-819A-93A2A7DA1688}"/>
   </bookViews>
   <sheets>
     <sheet name="illicit_crops" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="36">
   <si>
     <t>Year</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Desagregacion</t>
   </si>
   <si>
-    <t>Valor</t>
-  </si>
-  <si>
     <t>CONDENADO</t>
   </si>
   <si>
@@ -139,6 +136,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>g_cat</t>
   </si>
 </sst>
 </file>
@@ -551,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70AB46DD-20D3-440B-99F9-91FE58E5B111}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -567,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -753,7 +756,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1802,25 +1805,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1A74D6-370B-4AC6-8F28-994E4AD39B41}">
-  <dimension ref="A1:G179"/>
+  <dimension ref="A1:I179"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.6640625" style="9" customWidth="1"/>
     <col min="2" max="2" width="56.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="50.21875" style="9" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" style="9" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="9"/>
+    <col min="6" max="8" width="12.88671875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="7" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1828,22 +1831,28 @@
         <v>15</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>2018</v>
       </c>
@@ -1851,22 +1860,28 @@
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="9">
         <v>1</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="9">
+        <v>1</v>
+      </c>
+      <c r="H2" s="9">
+        <v>1</v>
+      </c>
+      <c r="I2" s="9">
         <v>16743</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2018</v>
       </c>
@@ -1874,22 +1889,28 @@
         <v>10</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="9">
         <v>1</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9">
         <v>7821</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>2018</v>
       </c>
@@ -1897,22 +1918,28 @@
         <v>10</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="9">
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="9">
+        <v>2</v>
+      </c>
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
         <v>20922</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2018</v>
       </c>
@@ -1920,22 +1947,28 @@
         <v>10</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="9">
         <v>1</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="9">
+        <v>2</v>
+      </c>
+      <c r="H5" s="9">
+        <v>2</v>
+      </c>
+      <c r="I5" s="9">
         <v>3642</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>2018</v>
       </c>
@@ -1943,22 +1976,28 @@
         <v>12</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="9">
         <v>2</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
         <v>568</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>2018</v>
       </c>
@@ -1966,22 +2005,28 @@
         <v>12</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="9">
         <v>2</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" s="9">
+        <v>1</v>
+      </c>
+      <c r="H7" s="9">
+        <v>2</v>
+      </c>
+      <c r="I7" s="9">
         <v>323</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>2018</v>
       </c>
@@ -1989,22 +2034,28 @@
         <v>12</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="9">
         <v>2</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="9">
+        <v>2</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
         <v>637</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>2018</v>
       </c>
@@ -2012,22 +2063,28 @@
         <v>12</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="9">
         <v>2</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" s="9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="9">
+        <v>2</v>
+      </c>
+      <c r="I9" s="9">
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>2018</v>
       </c>
@@ -2035,22 +2092,28 @@
         <v>11</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="9">
         <v>3</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" s="9">
+        <v>1</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9">
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>2018</v>
       </c>
@@ -2058,22 +2121,28 @@
         <v>11</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="9">
         <v>3</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" s="9">
+        <v>1</v>
+      </c>
+      <c r="H11" s="9">
+        <v>2</v>
+      </c>
+      <c r="I11" s="9">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>2018</v>
       </c>
@@ -2081,22 +2150,28 @@
         <v>11</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="9">
         <v>3</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" s="9">
+        <v>2</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1</v>
+      </c>
+      <c r="I12" s="9">
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>2018</v>
       </c>
@@ -2104,22 +2179,28 @@
         <v>11</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="9">
         <v>3</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G13" s="9">
+        <v>2</v>
+      </c>
+      <c r="H13" s="9">
+        <v>2</v>
+      </c>
+      <c r="I13" s="9">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>2018</v>
       </c>
@@ -2127,22 +2208,28 @@
         <v>13</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="9">
         <v>4</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" s="9">
+        <v>1</v>
+      </c>
+      <c r="H14" s="9">
+        <v>1</v>
+      </c>
+      <c r="I14" s="9">
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>2018</v>
       </c>
@@ -2150,22 +2237,28 @@
         <v>13</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="9">
         <v>4</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G15" s="9">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9">
+        <v>2</v>
+      </c>
+      <c r="I15" s="9">
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>2018</v>
       </c>
@@ -2173,22 +2266,28 @@
         <v>13</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="9">
         <v>4</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" s="9">
+        <v>2</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9">
         <v>391</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>2018</v>
       </c>
@@ -2196,22 +2295,28 @@
         <v>13</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="9">
         <v>4</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G17" s="9">
+        <v>2</v>
+      </c>
+      <c r="H17" s="9">
+        <v>2</v>
+      </c>
+      <c r="I17" s="9">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>2018</v>
       </c>
@@ -2219,22 +2324,28 @@
         <v>14</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="9">
         <v>5</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G18" s="9">
+        <v>1</v>
+      </c>
+      <c r="H18" s="9">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>2018</v>
       </c>
@@ -2242,22 +2353,28 @@
         <v>14</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="9">
         <v>5</v>
       </c>
       <c r="E19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="9">
+        <v>1</v>
+      </c>
+      <c r="H19" s="9">
+        <v>2</v>
+      </c>
+      <c r="I19" s="9">
         <v>19</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="9">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>2018</v>
       </c>
@@ -2265,22 +2382,28 @@
         <v>14</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="9">
         <v>5</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G20" s="9">
+        <v>2</v>
+      </c>
+      <c r="H20" s="9">
+        <v>1</v>
+      </c>
+      <c r="I20" s="9">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>2018</v>
       </c>
@@ -2288,31 +2411,37 @@
         <v>14</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="9">
         <v>5</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G21" s="9">
+        <v>2</v>
+      </c>
+      <c r="H21" s="9">
+        <v>2</v>
+      </c>
+      <c r="I21" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2454,7 +2583,7 @@
     <row r="178" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="179" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I21">
     <sortCondition ref="D2:D21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>